<commit_message>
add the format for fixed OD pairs
</commit_message>
<xml_diff>
--- a/simple_data/EXPLANATION.xlsx
+++ b/simple_data/EXPLANATION.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CTA-optimal-control-under-incidents\simple_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B282C08-BF01-41B3-AAA6-549A016E425F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B824D-22DF-4B52-928A-A9BA152FC905}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11940" activeTab="3" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11940" activeTab="1" xr2:uid="{1825468F-3913-41A2-9689-94FCDE51F798}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="4" r:id="rId1"/>
-    <sheet name="policy_num" sheetId="1" r:id="rId2"/>
-    <sheet name="policy" sheetId="2" r:id="rId3"/>
-    <sheet name="direction" sheetId="3" r:id="rId4"/>
-    <sheet name="arrivalTime" sheetId="5" r:id="rId5"/>
-    <sheet name="arrivalStationID" sheetId="6" r:id="rId6"/>
-    <sheet name="startTrainInfo" sheetId="7" r:id="rId7"/>
-    <sheet name="transferTime" sheetId="9" r:id="rId8"/>
+    <sheet name="fixOD" sheetId="10" r:id="rId2"/>
+    <sheet name="policy_num" sheetId="1" r:id="rId3"/>
+    <sheet name="policy" sheetId="2" r:id="rId4"/>
+    <sheet name="direction" sheetId="3" r:id="rId5"/>
+    <sheet name="arrivalTime" sheetId="5" r:id="rId6"/>
+    <sheet name="arrivalStationID" sheetId="6" r:id="rId7"/>
+    <sheet name="startTrainInfo" sheetId="7" r:id="rId8"/>
+    <sheet name="transferTime" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>stationID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -226,6 +227,30 @@
   </si>
   <si>
     <t>程序里会认为这个表里没覆盖到的站站对是在不同线路上的，需要transfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要按time升序排序以达到最大效率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>避免出现从自己到自己的OD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -615,7 +640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4331848-2BA8-4AC2-929A-520C1CE3094F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0"/>
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -717,6 +744,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9AF7CD-4EA7-4D92-81C9-C5F14D8EA680}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA90451-AF43-4586-8589-D683FC77F309}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -793,7 +964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A06958D-3E10-44DF-B5AA-81043F13CD0A}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -891,11 +1062,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A178DC-DEE4-47F5-935D-91472836669E}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+    <sheetView zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1005,7 +1176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E2EAB8-4C91-42DA-A785-B9C6D472A7C6}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -1381,7 +1552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FF9D8A-27B6-45CF-B9C7-0CE2AB549F98}">
   <dimension ref="A1:C32"/>
   <sheetViews>
@@ -1706,11 +1877,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C1F831-9559-482A-A6EE-7D70457D36F8}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F27"/>
     </sheetView>
   </sheetViews>
@@ -2294,7 +2465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7B84D8-7FF5-4E19-9919-9768BB2E536C}">
   <dimension ref="A1:D8"/>
   <sheetViews>

</xml_diff>